<commit_message>
created a base file, Test annotations Log in Method
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/userdata.xlsx
+++ b/src/test/java/TestData/userdata.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Login Credentials" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -395,7 +395,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>